<commit_message>
Refactoring data processing correlations
</commit_message>
<xml_diff>
--- a/experimental_data/GEC/Schnegg1986.xlsx
+++ b/experimental_data/GEC/Schnegg1986.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="107">
   <si>
     <t>Schnegg1986 – Quantitative Liver Function in the Elderly Assessed by GEC</t>
   </si>
@@ -218,6 +218,9 @@
     <t>Table 3</t>
   </si>
   <si>
+    <t>Age status</t>
+  </si>
+  <si>
     <t>n GEC</t>
   </si>
   <si>
@@ -261,6 +264,9 @@
   </si>
   <si>
     <t>Aminopyrine breath test [% dose x kg/mmoles CO2] SD</t>
+  </si>
+  <si>
+    <t>ageStatus</t>
   </si>
   <si>
     <t>nGEC</t>
@@ -610,7 +616,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1247,11 +1253,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="39605283"/>
-        <c:axId val="33484319"/>
+        <c:axId val="55071276"/>
+        <c:axId val="99577780"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="39605283"/>
+        <c:axId val="55071276"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1287,11 +1293,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="33484319"/>
+        <c:crossAx val="99577780"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="33484319"/>
+        <c:axId val="99577780"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
@@ -1328,7 +1334,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="39605283"/>
+        <c:crossAx val="55071276"/>
         <c:crossesAt val="0"/>
         <c:majorUnit val="2"/>
       </c:valAx>
@@ -1354,7 +1360,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1649,11 +1655,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="55883257"/>
-        <c:axId val="50949528"/>
+        <c:axId val="38028485"/>
+        <c:axId val="11591500"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="55883257"/>
+        <c:axId val="38028485"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="90"/>
@@ -1691,12 +1697,12 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="50949528"/>
+        <c:crossAx val="11591500"/>
         <c:crossesAt val="0"/>
         <c:majorUnit val="20"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="50949528"/>
+        <c:axId val="11591500"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2.5"/>
@@ -1734,7 +1740,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="55883257"/>
+        <c:crossAx val="38028485"/>
         <c:crossesAt val="0"/>
         <c:majorUnit val="1"/>
       </c:valAx>
@@ -1760,7 +1766,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2091,11 +2097,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="44514122"/>
-        <c:axId val="13963499"/>
+        <c:axId val="31928015"/>
+        <c:axId val="51323410"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="44514122"/>
+        <c:axId val="31928015"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="90"/>
@@ -2133,12 +2139,12 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="13963499"/>
+        <c:crossAx val="51323410"/>
         <c:crossesAt val="0"/>
         <c:majorUnit val="20"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="13963499"/>
+        <c:axId val="51323410"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2174,7 +2180,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="44514122"/>
+        <c:crossAx val="31928015"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -2205,14 +2211,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>730800</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>28440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>366840</xdr:colOff>
-      <xdr:row>90</xdr:row>
-      <xdr:rowOff>146160</xdr:rowOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>128880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2244,14 +2250,14 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>465120</xdr:colOff>
-      <xdr:row>70</xdr:row>
-      <xdr:rowOff>125640</xdr:rowOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>108720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>358920</xdr:colOff>
-      <xdr:row>93</xdr:row>
-      <xdr:rowOff>62640</xdr:rowOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2283,14 +2289,14 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>467280</xdr:colOff>
-      <xdr:row>92</xdr:row>
-      <xdr:rowOff>36720</xdr:rowOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>19440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>81720</xdr:colOff>
-      <xdr:row>116</xdr:row>
-      <xdr:rowOff>78840</xdr:rowOff>
+      <xdr:row>118</xdr:row>
+      <xdr:rowOff>61560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2328,8 +2334,8 @@
     <xdr:to>
       <xdr:col>30</xdr:col>
       <xdr:colOff>758880</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>41760</xdr:rowOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>24480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2361,14 +2367,14 @@
     <xdr:from>
       <xdr:col>22</xdr:col>
       <xdr:colOff>328680</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>155880</xdr:rowOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>138600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>30</xdr:col>
       <xdr:colOff>738000</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>5040</xdr:rowOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>150480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2400,14 +2406,14 @@
     <xdr:from>
       <xdr:col>19</xdr:col>
       <xdr:colOff>575280</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>3600</xdr:rowOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>149040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
       <xdr:colOff>136800</xdr:colOff>
-      <xdr:row>74</xdr:row>
-      <xdr:rowOff>87120</xdr:rowOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>69840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2439,14 +2445,14 @@
     <xdr:from>
       <xdr:col>28</xdr:col>
       <xdr:colOff>459360</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>158760</xdr:rowOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>141840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>33</xdr:col>
       <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>79</xdr:row>
-      <xdr:rowOff>51480</xdr:rowOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>34560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2469,14 +2475,14 @@
     <xdr:from>
       <xdr:col>25</xdr:col>
       <xdr:colOff>809280</xdr:colOff>
-      <xdr:row>72</xdr:row>
-      <xdr:rowOff>48240</xdr:rowOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>30960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>31</xdr:col>
       <xdr:colOff>405360</xdr:colOff>
-      <xdr:row>91</xdr:row>
-      <xdr:rowOff>16920</xdr:rowOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>162000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2499,14 +2505,14 @@
     <xdr:from>
       <xdr:col>21</xdr:col>
       <xdr:colOff>673920</xdr:colOff>
-      <xdr:row>74</xdr:row>
-      <xdr:rowOff>147240</xdr:rowOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>129960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>460800</xdr:colOff>
-      <xdr:row>93</xdr:row>
-      <xdr:rowOff>37080</xdr:rowOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>20160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2535,8 +2541,8 @@
   </sheetPr>
   <dimension ref="A1:AA130"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A39" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M30" activeCellId="0" sqref="M30:Q73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3853,109 +3859,115 @@
       <c r="P20" s="11"/>
       <c r="Q20" s="11"/>
     </row>
-    <row r="21" customFormat="false" ht="79.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="8" t="s">
+        <v>67</v>
+      </c>
       <c r="B21" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="J21" s="8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="K21" s="8" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="L21" s="8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="M21" s="8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="N21" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="O21" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="P21" s="8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="Q21" s="8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="10" t="s">
+        <v>83</v>
+      </c>
       <c r="B22" s="10" t="s">
         <v>33</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="F22" s="10" t="s">
         <v>52</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="J22" s="10" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="K22" s="10" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="L22" s="10" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="M22" s="10" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="N22" s="10" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="O22" s="10" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="P22" s="10" t="s">
         <v>46</v>
       </c>
       <c r="Q22" s="10" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="12" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>60</v>
@@ -4008,7 +4020,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="12" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>60</v>
@@ -4061,7 +4073,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="12" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>60</v>
@@ -4114,13 +4126,13 @@
     </row>
     <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="66.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4134,7 +4146,7 @@
         <v>9</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E29" s="8" t="s">
         <v>6</v>
@@ -4149,7 +4161,7 @@
         <v>9</v>
       </c>
       <c r="J29" s="8" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K29" s="8" t="s">
         <v>8</v>
@@ -4164,7 +4176,7 @@
         <v>9</v>
       </c>
       <c r="P29" s="8" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="Q29" s="8" t="s">
         <v>8</v>
@@ -4181,7 +4193,7 @@
         <v>36</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E30" s="10" t="s">
         <v>33</v>
@@ -4196,7 +4208,7 @@
         <v>36</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="K30" s="10" t="s">
         <v>35</v>
@@ -4222,7 +4234,7 @@
         <v>59</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C31" s="0" t="n">
         <v>15.773049</v>
@@ -4237,7 +4249,7 @@
         <v>59</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I31" s="0" t="n">
         <v>24.745762</v>
@@ -4252,7 +4264,7 @@
         <v>59</v>
       </c>
       <c r="N31" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="O31" s="0" t="n">
         <v>18.177933</v>
@@ -4269,7 +4281,7 @@
         <v>59</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C32" s="0" t="n">
         <v>18.609928</v>
@@ -4284,7 +4296,7 @@
         <v>59</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I32" s="0" t="n">
         <v>27.00565</v>
@@ -4299,7 +4311,7 @@
         <v>59</v>
       </c>
       <c r="N32" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="O32" s="0" t="n">
         <v>22.092466</v>
@@ -4316,7 +4328,7 @@
         <v>59</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C33" s="0" t="n">
         <v>19.631207</v>
@@ -4331,7 +4343,7 @@
         <v>59</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I33" s="0" t="n">
         <v>27.79661</v>
@@ -4346,7 +4358,7 @@
         <v>59</v>
       </c>
       <c r="N33" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="O33" s="0" t="n">
         <v>20.1282</v>
@@ -4363,7 +4375,7 @@
         <v>59</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C34" s="0" t="n">
         <v>19.74468</v>
@@ -4378,7 +4390,7 @@
         <v>59</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I34" s="0" t="n">
         <v>28.58757</v>
@@ -4393,7 +4405,7 @@
         <v>59</v>
       </c>
       <c r="N34" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="O34" s="0" t="n">
         <v>23.340578</v>
@@ -4410,7 +4422,7 @@
         <v>59</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C35" s="0" t="n">
         <v>19.74468</v>
@@ -4425,7 +4437,7 @@
         <v>59</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I35" s="0" t="n">
         <v>29.83051</v>
@@ -4440,7 +4452,7 @@
         <v>59</v>
       </c>
       <c r="N35" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="O35" s="0" t="n">
         <v>24.555534</v>
@@ -4457,7 +4469,7 @@
         <v>59</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C36" s="0" t="n">
         <v>20.652483</v>
@@ -4472,7 +4484,7 @@
         <v>59</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I36" s="0" t="n">
         <v>32.542374</v>
@@ -4487,7 +4499,7 @@
         <v>59</v>
       </c>
       <c r="N36" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="O36" s="0" t="n">
         <v>25.05581</v>
@@ -4504,7 +4516,7 @@
         <v>59</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C37" s="0" t="n">
         <v>21.67376</v>
@@ -4519,7 +4531,7 @@
         <v>59</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I37" s="0" t="n">
         <v>23.728813</v>
@@ -4534,7 +4546,7 @@
         <v>59</v>
       </c>
       <c r="N37" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="O37" s="0" t="n">
         <v>25.39547</v>
@@ -4551,7 +4563,7 @@
         <v>59</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C38" s="0" t="n">
         <v>22.695036</v>
@@ -4566,7 +4578,7 @@
         <v>59</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I38" s="0" t="n">
         <v>27.79661</v>
@@ -4581,7 +4593,7 @@
         <v>59</v>
       </c>
       <c r="N38" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="O38" s="0" t="n">
         <v>26.092466</v>
@@ -4598,7 +4610,7 @@
         <v>59</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C39" s="0" t="n">
         <v>23.716312</v>
@@ -4613,7 +4625,7 @@
         <v>59</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I39" s="0" t="n">
         <v>22.146893</v>
@@ -4628,7 +4640,7 @@
         <v>59</v>
       </c>
       <c r="N39" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="O39" s="0" t="n">
         <v>27.286057</v>
@@ -4645,7 +4657,7 @@
         <v>59</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C40" s="0" t="n">
         <v>23.943262</v>
@@ -4660,7 +4672,7 @@
         <v>59</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I40" s="0" t="n">
         <v>24.632769</v>
@@ -4675,7 +4687,7 @@
         <v>59</v>
       </c>
       <c r="N40" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="O40" s="0" t="n">
         <v>27.109964</v>
@@ -4692,7 +4704,7 @@
         <v>59</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C41" s="0" t="n">
         <v>21.560284</v>
@@ -4707,7 +4719,7 @@
         <v>59</v>
       </c>
       <c r="H41" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I41" s="0" t="n">
         <v>26.779661</v>
@@ -4722,7 +4734,7 @@
         <v>59</v>
       </c>
       <c r="N41" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="O41" s="0" t="n">
         <v>27.268373</v>
@@ -4739,7 +4751,7 @@
         <v>59</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C42" s="0" t="n">
         <v>21.333334</v>
@@ -4754,7 +4766,7 @@
         <v>59</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I42" s="0" t="n">
         <v>25.649717</v>
@@ -4769,7 +4781,7 @@
         <v>59</v>
       </c>
       <c r="N42" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="O42" s="0" t="n">
         <v>30.375391</v>
@@ -4786,7 +4798,7 @@
         <v>59</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C43" s="0" t="n">
         <v>21.67376</v>
@@ -4801,7 +4813,7 @@
         <v>59</v>
       </c>
       <c r="H43" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I43" s="0" t="n">
         <v>28.58757</v>
@@ -4816,7 +4828,7 @@
         <v>59</v>
       </c>
       <c r="N43" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="O43" s="0" t="n">
         <v>29.419783</v>
@@ -4833,7 +4845,7 @@
         <v>59</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C44" s="0" t="n">
         <v>23.602837</v>
@@ -4848,7 +4860,7 @@
         <v>59</v>
       </c>
       <c r="H44" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I44" s="0" t="n">
         <v>34.915253</v>
@@ -4863,7 +4875,7 @@
         <v>59</v>
       </c>
       <c r="N44" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="O44" s="0" t="n">
         <v>35.244797</v>
@@ -4880,7 +4892,7 @@
         <v>59</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C45" s="0" t="n">
         <v>24.51064</v>
@@ -4895,7 +4907,7 @@
         <v>59</v>
       </c>
       <c r="H45" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I45" s="0" t="n">
         <v>33.559322</v>
@@ -4910,7 +4922,7 @@
         <v>59</v>
       </c>
       <c r="N45" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="O45" s="0" t="n">
         <v>35.235954</v>
@@ -4927,7 +4939,7 @@
         <v>59</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C46" s="0" t="n">
         <v>25.41844</v>
@@ -4942,7 +4954,7 @@
         <v>59</v>
       </c>
       <c r="H46" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I46" s="0" t="n">
         <v>35.028248</v>
@@ -4957,7 +4969,7 @@
         <v>59</v>
       </c>
       <c r="N46" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="O46" s="0" t="n">
         <v>33.313686</v>
@@ -4974,7 +4986,7 @@
         <v>59</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C47" s="0" t="n">
         <v>24.624113</v>
@@ -4989,7 +5001,7 @@
         <v>59</v>
       </c>
       <c r="H47" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I47" s="0" t="n">
         <v>41.920902</v>
@@ -5004,7 +5016,7 @@
         <v>59</v>
       </c>
       <c r="N47" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="O47" s="0" t="n">
         <v>33.310738</v>
@@ -5021,7 +5033,7 @@
         <v>59</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C48" s="0" t="n">
         <v>23.716312</v>
@@ -5036,7 +5048,7 @@
         <v>59</v>
       </c>
       <c r="H48" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I48" s="0" t="n">
         <v>43.954803</v>
@@ -5051,7 +5063,7 @@
         <v>59</v>
       </c>
       <c r="N48" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="O48" s="0" t="n">
         <v>34.129307</v>
@@ -5068,7 +5080,7 @@
         <v>59</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C49" s="0" t="n">
         <v>22.695036</v>
@@ -5083,7 +5095,7 @@
         <v>59</v>
       </c>
       <c r="H49" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I49" s="0" t="n">
         <v>45.536724</v>
@@ -5098,7 +5110,7 @@
         <v>59</v>
       </c>
       <c r="N49" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="O49" s="0" t="n">
         <v>35.12912</v>
@@ -5115,7 +5127,7 @@
         <v>59</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C50" s="0" t="n">
         <v>21.90071</v>
@@ -5130,7 +5142,7 @@
         <v>59</v>
       </c>
       <c r="H50" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I50" s="0" t="n">
         <v>53.78531</v>
@@ -5145,7 +5157,7 @@
         <v>59</v>
       </c>
       <c r="N50" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="O50" s="0" t="n">
         <v>39.289005</v>
@@ -5162,7 +5174,7 @@
         <v>59</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C51" s="0" t="n">
         <v>22.58156</v>
@@ -5177,7 +5189,7 @@
         <v>59</v>
       </c>
       <c r="H51" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I51" s="0" t="n">
         <v>53.446327</v>
@@ -5192,7 +5204,7 @@
         <v>59</v>
       </c>
       <c r="N51" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="O51" s="0" t="n">
         <v>40.342606</v>
@@ -5209,7 +5221,7 @@
         <v>59</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C52" s="0" t="n">
         <v>22.80851</v>
@@ -5224,7 +5236,7 @@
         <v>59</v>
       </c>
       <c r="H52" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I52" s="0" t="n">
         <v>50.847458</v>
@@ -5239,7 +5251,7 @@
         <v>59</v>
       </c>
       <c r="N52" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="O52" s="0" t="n">
         <v>47.27869</v>
@@ -5256,7 +5268,7 @@
         <v>59</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C53" s="0" t="n">
         <v>21.106382</v>
@@ -5271,7 +5283,7 @@
         <v>59</v>
       </c>
       <c r="H53" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I53" s="0" t="n">
         <v>50.847458</v>
@@ -5286,7 +5298,7 @@
         <v>59</v>
       </c>
       <c r="N53" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="O53" s="0" t="n">
         <v>52.374287</v>
@@ -5303,7 +5315,7 @@
         <v>59</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C54" s="0" t="n">
         <v>21.67376</v>
@@ -5318,7 +5330,7 @@
         <v>59</v>
       </c>
       <c r="H54" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I54" s="0" t="n">
         <v>59.435028</v>
@@ -5333,7 +5345,7 @@
         <v>59</v>
       </c>
       <c r="N54" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="O54" s="0" t="n">
         <v>50.434334</v>
@@ -5350,7 +5362,7 @@
         <v>59</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C55" s="0" t="n">
         <v>22.014185</v>
@@ -5365,7 +5377,7 @@
         <v>59</v>
       </c>
       <c r="H55" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I55" s="0" t="n">
         <v>57.627117</v>
@@ -5380,7 +5392,7 @@
         <v>59</v>
       </c>
       <c r="N55" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="O55" s="0" t="n">
         <v>57.098545</v>
@@ -5397,7 +5409,7 @@
         <v>59</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C56" s="0" t="n">
         <v>21.787233</v>
@@ -5412,7 +5424,7 @@
         <v>59</v>
       </c>
       <c r="H56" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I56" s="0" t="n">
         <v>55.932205</v>
@@ -5427,7 +5439,7 @@
         <v>59</v>
       </c>
       <c r="N56" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="O56" s="0" t="n">
         <v>58.421074</v>
@@ -5444,7 +5456,7 @@
         <v>59</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C57" s="0" t="n">
         <v>21.90071</v>
@@ -5459,7 +5471,7 @@
         <v>59</v>
       </c>
       <c r="H57" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I57" s="0" t="n">
         <v>61.80791</v>
@@ -5474,7 +5486,7 @@
         <v>59</v>
       </c>
       <c r="N57" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="O57" s="0" t="n">
         <v>63.176277</v>
@@ -5491,7 +5503,7 @@
         <v>59</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C58" s="0" t="n">
         <v>22.58156</v>
@@ -5506,7 +5518,7 @@
         <v>59</v>
       </c>
       <c r="H58" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I58" s="0" t="n">
         <v>62.59887</v>
@@ -5521,7 +5533,7 @@
         <v>59</v>
       </c>
       <c r="N58" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="O58" s="0" t="n">
         <v>61.24369</v>
@@ -5538,7 +5550,7 @@
         <v>59</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C59" s="0" t="n">
         <v>22.014185</v>
@@ -5553,7 +5565,7 @@
         <v>59</v>
       </c>
       <c r="H59" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I59" s="0" t="n">
         <v>70.62147</v>
@@ -5568,7 +5580,7 @@
         <v>59</v>
       </c>
       <c r="N59" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="O59" s="0" t="n">
         <v>62.270767</v>
@@ -5585,7 +5597,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C60" s="0" t="n">
         <v>22.80851</v>
@@ -5600,7 +5612,7 @@
         <v>59</v>
       </c>
       <c r="H60" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I60" s="0" t="n">
         <v>76.94915</v>
@@ -5615,7 +5627,7 @@
         <v>59</v>
       </c>
       <c r="N60" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="O60" s="0" t="n">
         <v>63.63087</v>
@@ -5632,7 +5644,7 @@
         <v>59</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C61" s="0" t="n">
         <v>22.695036</v>
@@ -5647,7 +5659,7 @@
         <v>59</v>
       </c>
       <c r="H61" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I61" s="0" t="n">
         <v>75.81921</v>
@@ -5662,7 +5674,7 @@
         <v>59</v>
       </c>
       <c r="N61" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="O61" s="0" t="n">
         <v>71.27574</v>
@@ -5679,7 +5691,7 @@
         <v>59</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C62" s="0" t="n">
         <v>23.716312</v>
@@ -5694,7 +5706,7 @@
         <v>59</v>
       </c>
       <c r="H62" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I62" s="0" t="n">
         <v>74.57627</v>
@@ -5709,7 +5721,7 @@
         <v>59</v>
       </c>
       <c r="N62" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="O62" s="0" t="n">
         <v>80.20188</v>
@@ -5726,7 +5738,7 @@
         <v>59</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C63" s="0" t="n">
         <v>23.829786</v>
@@ -5741,7 +5753,7 @@
         <v>59</v>
       </c>
       <c r="H63" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I63" s="0" t="n">
         <v>70.62147</v>
@@ -5756,7 +5768,7 @@
         <v>59</v>
       </c>
       <c r="N63" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="O63" s="0" t="n">
         <v>81.220116</v>
@@ -5773,7 +5785,7 @@
         <v>59</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C64" s="0" t="n">
         <v>23.716312</v>
@@ -5788,7 +5800,7 @@
         <v>59</v>
       </c>
       <c r="H64" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I64" s="0" t="n">
         <v>81.694916</v>
@@ -5803,7 +5815,7 @@
         <v>59</v>
       </c>
       <c r="N64" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="O64" s="0" t="n">
         <v>77.240005</v>
@@ -5820,7 +5832,7 @@
         <v>59</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C65" s="0" t="n">
         <v>23.48936</v>
@@ -5835,7 +5847,7 @@
         <v>59</v>
       </c>
       <c r="H65" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I65" s="0" t="n">
         <v>84.745766</v>
@@ -5850,7 +5862,7 @@
         <v>59</v>
       </c>
       <c r="N65" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="O65" s="0" t="n">
         <v>70.8322</v>
@@ -5867,7 +5879,7 @@
         <v>59</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C66" s="0" t="n">
         <v>23.262411</v>
@@ -5882,7 +5894,7 @@
         <v>59</v>
       </c>
       <c r="H66" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I66" s="0" t="n">
         <v>80.56497</v>
@@ -5897,7 +5909,7 @@
         <v>59</v>
       </c>
       <c r="N66" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="O66" s="0" t="n">
         <v>70.97071</v>
@@ -5914,7 +5926,7 @@
         <v>59</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C67" s="0" t="n">
         <v>23.716312</v>
@@ -5929,7 +5941,7 @@
         <v>59</v>
       </c>
       <c r="H67" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I67" s="0" t="n">
         <v>87.68362</v>
@@ -5944,7 +5956,7 @@
         <v>59</v>
       </c>
       <c r="N67" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="O67" s="0" t="n">
         <v>75.132805</v>
@@ -5961,7 +5973,7 @@
         <v>59</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C68" s="0" t="n">
         <v>22.921986</v>
@@ -5976,7 +5988,7 @@
         <v>59</v>
       </c>
       <c r="N68" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="O68" s="0" t="n">
         <v>76.16725</v>
@@ -5993,7 +6005,7 @@
         <v>59</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C69" s="0" t="n">
         <v>23.148935</v>
@@ -6008,7 +6020,7 @@
         <v>59</v>
       </c>
       <c r="N69" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="O69" s="0" t="n">
         <v>78.03352</v>
@@ -6025,7 +6037,7 @@
         <v>59</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C70" s="0" t="n">
         <v>24.624113</v>
@@ -6040,7 +6052,7 @@
         <v>59</v>
       </c>
       <c r="N70" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="O70" s="0" t="n">
         <v>80.95856</v>
@@ -6057,7 +6069,7 @@
         <v>59</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C71" s="0" t="n">
         <v>24.170214</v>
@@ -6072,7 +6084,7 @@
         <v>59</v>
       </c>
       <c r="N71" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="O71" s="0" t="n">
         <v>82.1853</v>
@@ -6089,7 +6101,7 @@
         <v>59</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C72" s="0" t="n">
         <v>24.737589</v>
@@ -6104,7 +6116,7 @@
         <v>59</v>
       </c>
       <c r="N72" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="O72" s="0" t="n">
         <v>88.2063</v>
@@ -6121,7 +6133,7 @@
         <v>59</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C73" s="0" t="n">
         <v>25.304964</v>
@@ -6136,7 +6148,7 @@
         <v>59</v>
       </c>
       <c r="N73" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="O73" s="0" t="n">
         <v>85.0816</v>
@@ -6153,7 +6165,7 @@
         <v>59</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C74" s="0" t="n">
         <v>25.64539</v>
@@ -6170,7 +6182,7 @@
         <v>59</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C75" s="0" t="n">
         <v>25.41844</v>
@@ -6187,7 +6199,7 @@
         <v>59</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C76" s="0" t="n">
         <v>26.780142</v>
@@ -6204,7 +6216,7 @@
         <v>59</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C77" s="0" t="n">
         <v>25.758865</v>
@@ -6221,7 +6233,7 @@
         <v>59</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C78" s="0" t="n">
         <v>25.078014</v>
@@ -6238,7 +6250,7 @@
         <v>59</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C79" s="0" t="n">
         <v>24.624113</v>
@@ -6255,7 +6267,7 @@
         <v>59</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C80" s="0" t="n">
         <v>24.624113</v>
@@ -6272,7 +6284,7 @@
         <v>59</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C81" s="0" t="n">
         <v>24.283688</v>
@@ -6289,7 +6301,7 @@
         <v>59</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C82" s="0" t="n">
         <v>24.624113</v>
@@ -6306,7 +6318,7 @@
         <v>59</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C83" s="0" t="n">
         <v>25.531916</v>
@@ -6323,7 +6335,7 @@
         <v>59</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C84" s="0" t="n">
         <v>27.687943</v>
@@ -6340,7 +6352,7 @@
         <v>59</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C85" s="0" t="n">
         <v>26.893618</v>
@@ -6357,7 +6369,7 @@
         <v>59</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C86" s="0" t="n">
         <v>26.666666</v>
@@ -6374,7 +6386,7 @@
         <v>59</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C87" s="0" t="n">
         <v>26.893618</v>
@@ -6391,7 +6403,7 @@
         <v>59</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C88" s="0" t="n">
         <v>26.893618</v>
@@ -6408,7 +6420,7 @@
         <v>59</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C89" s="0" t="n">
         <v>30.751774</v>
@@ -6425,7 +6437,7 @@
         <v>59</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C90" s="0" t="n">
         <v>32.567375</v>
@@ -6442,7 +6454,7 @@
         <v>59</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C91" s="0" t="n">
         <v>28.822695</v>
@@ -6459,7 +6471,7 @@
         <v>59</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C92" s="0" t="n">
         <v>29.957447</v>
@@ -6476,7 +6488,7 @@
         <v>59</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C93" s="0" t="n">
         <v>30.638298</v>
@@ -6493,7 +6505,7 @@
         <v>59</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C94" s="0" t="n">
         <v>32.567375</v>
@@ -6510,7 +6522,7 @@
         <v>59</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C95" s="0" t="n">
         <v>32.113476</v>
@@ -6527,7 +6539,7 @@
         <v>59</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C96" s="0" t="n">
         <v>36.539005</v>
@@ -6544,7 +6556,7 @@
         <v>59</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C97" s="0" t="n">
         <v>37.67376</v>
@@ -6561,7 +6573,7 @@
         <v>59</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C98" s="0" t="n">
         <v>37.90071</v>
@@ -6578,7 +6590,7 @@
         <v>59</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C99" s="0" t="n">
         <v>38.695034</v>
@@ -6595,7 +6607,7 @@
         <v>59</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C100" s="0" t="n">
         <v>38.581562</v>
@@ -6612,7 +6624,7 @@
         <v>59</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C101" s="0" t="n">
         <v>39.716312</v>
@@ -6629,7 +6641,7 @@
         <v>59</v>
       </c>
       <c r="B102" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C102" s="0" t="n">
         <v>43.574467</v>
@@ -6646,7 +6658,7 @@
         <v>59</v>
       </c>
       <c r="B103" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C103" s="0" t="n">
         <v>44.70922</v>
@@ -6663,7 +6675,7 @@
         <v>59</v>
       </c>
       <c r="B104" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C104" s="0" t="n">
         <v>47.77305</v>
@@ -6680,7 +6692,7 @@
         <v>59</v>
       </c>
       <c r="B105" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C105" s="0" t="n">
         <v>49.70213</v>
@@ -6697,7 +6709,7 @@
         <v>59</v>
       </c>
       <c r="B106" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C106" s="0" t="n">
         <v>51.51773</v>
@@ -6714,7 +6726,7 @@
         <v>59</v>
       </c>
       <c r="B107" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C107" s="0" t="n">
         <v>56.51064</v>
@@ -6731,7 +6743,7 @@
         <v>59</v>
       </c>
       <c r="B108" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C108" s="0" t="n">
         <v>57.64539</v>
@@ -6748,7 +6760,7 @@
         <v>59</v>
       </c>
       <c r="B109" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C109" s="0" t="n">
         <v>60.595745</v>
@@ -6765,7 +6777,7 @@
         <v>59</v>
       </c>
       <c r="B110" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C110" s="0" t="n">
         <v>62.638298</v>
@@ -6782,7 +6794,7 @@
         <v>59</v>
       </c>
       <c r="B111" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C111" s="0" t="n">
         <v>62.638298</v>
@@ -6799,7 +6811,7 @@
         <v>59</v>
       </c>
       <c r="B112" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C112" s="0" t="n">
         <v>70.35461</v>
@@ -6816,7 +6828,7 @@
         <v>59</v>
       </c>
       <c r="B113" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C113" s="0" t="n">
         <v>70.46809</v>
@@ -6833,7 +6845,7 @@
         <v>59</v>
       </c>
       <c r="B114" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C114" s="0" t="n">
         <v>70.58156</v>
@@ -6850,7 +6862,7 @@
         <v>59</v>
       </c>
       <c r="B115" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C115" s="0" t="n">
         <v>74.43971</v>
@@ -6867,7 +6879,7 @@
         <v>59</v>
       </c>
       <c r="B116" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C116" s="0" t="n">
         <v>75.34752</v>
@@ -6884,7 +6896,7 @@
         <v>59</v>
       </c>
       <c r="B117" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C117" s="0" t="n">
         <v>76.59574</v>
@@ -6901,7 +6913,7 @@
         <v>59</v>
       </c>
       <c r="B118" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C118" s="0" t="n">
         <v>77.39007</v>
@@ -6918,7 +6930,7 @@
         <v>59</v>
       </c>
       <c r="B119" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C119" s="0" t="n">
         <v>79.5461</v>
@@ -6935,7 +6947,7 @@
         <v>59</v>
       </c>
       <c r="B120" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C120" s="0" t="n">
         <v>81.702126</v>
@@ -6952,7 +6964,7 @@
         <v>59</v>
       </c>
       <c r="B121" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C121" s="0" t="n">
         <v>84.53901</v>
@@ -6969,7 +6981,7 @@
         <v>59</v>
       </c>
       <c r="B122" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C122" s="0" t="n">
         <v>80.680855</v>
@@ -6986,7 +6998,7 @@
         <v>59</v>
       </c>
       <c r="B123" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C123" s="0" t="n">
         <v>80.567375</v>
@@ -7003,7 +7015,7 @@
         <v>59</v>
       </c>
       <c r="B124" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C124" s="0" t="n">
         <v>88.510635</v>

</xml_diff>